<commit_message>
changes in interpolation function
</commit_message>
<xml_diff>
--- a/mid_size_industrial_prices.xlsx
+++ b/mid_size_industrial_prices.xlsx
@@ -411,7 +411,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>12.735</v>
+        <v>10.5525</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -419,7 +419,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>12.69</v>
+        <v>11.325</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -427,7 +427,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>12.32</v>
+        <v>10.64</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -435,7 +435,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>13.355</v>
+        <v>11.3175</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -443,7 +443,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>15.215</v>
+        <v>12.6425</v>
       </c>
     </row>
   </sheetData>

</xml_diff>